<commit_message>
1.Excel + func. testing + needed files 2.Funcional testing in OOP + working webdriver wo error
</commit_message>
<xml_diff>
--- a/excel/Configuration.xlsx
+++ b/excel/Configuration.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\PycharmProjects\Testing-tool\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F409D4F-034E-429A-A7D3-48759EB74A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -18,12 +24,43 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>https://www.seznam.cz</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -46,14 +83,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +370,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{FF333463-199F-48CD-85D2-D95144F04579}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
+ searchbar; +whatsearch; +button click
</commit_message>
<xml_diff>
--- a/excel/Configuration.xlsx
+++ b/excel/Configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\PycharmProjects\Testing-tool\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD26A8F-1C09-4122-9B0E-9CEF3E1D47F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5397BE13-3381-41DF-95DB-31900071CF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>URL</t>
   </si>
@@ -46,13 +46,25 @@
   </si>
   <si>
     <t>Search</t>
+  </si>
+  <si>
+    <t>Whatsearch</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>Mobil</t>
+  </si>
+  <si>
+    <t>//*[@id="rootHead"]/form/button[2]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +79,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -90,9 +109,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
@@ -374,15 +394,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -393,10 +416,16 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -406,12 +435,18 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{FF333463-199F-48CD-85D2-D95144F04579}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding and editing comment and warnings
</commit_message>
<xml_diff>
--- a/excel/Configuration.xlsx
+++ b/excel/Configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\PycharmProjects\Testing-tool\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5397BE13-3381-41DF-95DB-31900071CF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC8EFC6-BCC2-4E0D-B95A-EFE6D5ECD4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>URL</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Search</t>
   </si>
   <si>
-    <t>Whatsearch</t>
-  </si>
-  <si>
     <t>Button</t>
   </si>
   <si>
@@ -58,6 +55,9 @@
   </si>
   <si>
     <t>//*[@id="rootHead"]/form/button[2]</t>
+  </si>
+  <si>
+    <t>XPath</t>
   </si>
 </sst>
 </file>
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -405,7 +405,7 @@
     <col min="4" max="4" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -419,27 +419,35 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C4" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Function code - excel import/export ok, test_case exceptions ok, executions ok To do - import multiple excels, export results for multiple excels to one excel
</commit_message>
<xml_diff>
--- a/excel/Configuration.xlsx
+++ b/excel/Configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\PycharmProjects\Testing-tool\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0535A8-7E14-4B3E-9377-5D0E5CE69ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20306FB3-BE5D-45EE-8B0D-0D4A67447F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4524" yWindow="1848" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -25,61 +25,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
   <si>
     <t>URL</t>
   </si>
   <si>
-    <t>Browser</t>
-  </si>
-  <si>
-    <t>Chrome</t>
+    <t>Wait</t>
   </si>
   <si>
     <t>End</t>
   </si>
   <si>
-    <t>https://www.heureka.cz</t>
-  </si>
-  <si>
-    <t>//*[@id="rootHead"]/form/input</t>
-  </si>
-  <si>
-    <t>Search</t>
-  </si>
-  <si>
     <t>Button</t>
   </si>
   <si>
-    <t>Mobil</t>
-  </si>
-  <si>
-    <t>//*[@id="rootHead"]/form/button[2]</t>
-  </si>
-  <si>
-    <t>XPath</t>
-  </si>
-  <si>
-    <t>Class</t>
-  </si>
-  <si>
-    <t>Select</t>
-  </si>
-  <si>
-    <t>c-accordion__button c-filter__title</t>
-  </si>
-  <si>
-    <t>Operační systém</t>
-  </si>
-  <si>
-    <t>Back</t>
+    <t>https://www.heureka.cz/</t>
+  </si>
+  <si>
+    <t>LINK</t>
+  </si>
+  <si>
+    <t>Co teď frčí</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +80,18 @@
       <name val="Consolas"/>
       <family val="3"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF94558D"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -124,10 +115,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
@@ -409,84 +403,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="4" max="4" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
+      <c r="D2" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+    <row r="3" spans="1:11">
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
+    <row r="4" spans="1:11">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{64446228-1F49-4EFD-8327-E7ED6185FF4B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>